<commit_message>
updating repo with my info
</commit_message>
<xml_diff>
--- a/data/cv_data.xlsx
+++ b/data/cv_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruybal.s/Documents/SR/cv/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwn351\Documents\Repositories\cv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542540B6-EB0F-514D-9FE0-614DA14B502D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34156F65-AD4A-4BDB-AE40-B475C159EAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15760" activeTab="1" xr2:uid="{70653332-357D-C843-A68B-418AF4257DE2}"/>
+    <workbookView xWindow="2955" yWindow="2985" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{70653332-357D-C843-A68B-418AF4257DE2}"/>
   </bookViews>
   <sheets>
     <sheet name="appointments" sheetId="1" r:id="rId1"/>
@@ -329,21 +329,9 @@
     <t>degree</t>
   </si>
   <si>
-    <t>Study Abroad Program (Spring 2011)</t>
-  </si>
-  <si>
-    <t>Maastricht University</t>
-  </si>
-  <si>
-    <t>Maastricht, Netherlands</t>
-  </si>
-  <si>
     <t>Undertook courses in immunology, human physiology and public health policymaking</t>
   </si>
   <si>
-    <t>B.A. Biology</t>
-  </si>
-  <si>
     <t>The Colorado College</t>
   </si>
   <si>
@@ -356,12 +344,6 @@
     <t>Recipient of the James Wilkes Memorial Prize in Biology (2011) awarded to the most outstanding undergraduate minority student in Biology</t>
   </si>
   <si>
-    <t>Recipient of the Venture Grant (2012) awarded to students with academic merit to support innovative project proposals</t>
-  </si>
-  <si>
-    <t>Ph.D. Genetic Epidemiology</t>
-  </si>
-  <si>
     <t>Recipient of the Melbourne International Engagement Award and Melbourne International Fee Remission Scholarship (2014-2018) awarded to a limited number of international students based on academic merit to cover full tuition and living costs</t>
   </si>
   <si>
@@ -1140,13 +1122,31 @@
   </si>
   <si>
     <t>Awarded A\$10,000 as AI for the project: Superstars in STEM High School Program</t>
+  </si>
+  <si>
+    <t>Brock University</t>
+  </si>
+  <si>
+    <t>B.Sc. Biomedical Sciences</t>
+  </si>
+  <si>
+    <t>M.Sc. Applied Health Sciences</t>
+  </si>
+  <si>
+    <t>Ph.D. Health Biosciences</t>
+  </si>
+  <si>
+    <t>St. Catharines, Canada</t>
+  </si>
+  <si>
+    <t>\href{https://dr.library.brocku.ca/handle/10464/16382}{Thesis: Sclerostin influences body composition adaptations to exercise training}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1183,14 +1183,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1511,12 +1509,12 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1536,7 +1534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1554,7 +1552,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1572,7 +1570,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1590,7 +1588,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1608,7 +1606,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1639,11 +1637,11 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
@@ -1655,40 +1653,40 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="B2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D2">
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D3">
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1697,26 +1695,26 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="C5" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D5">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B6" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1725,12 +1723,12 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B7" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1739,12 +1737,12 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1753,12 +1751,12 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1776,16 +1774,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCD460E-1FF0-2C43-8A33-221816BDB936}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1799,7 +1797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1813,7 +1811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1827,7 +1825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1855,7 +1853,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1869,7 +1867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1883,21 +1881,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D8" t="s">
         <v>359</v>
       </c>
-      <c r="D8" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1911,7 +1909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1925,7 +1923,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1939,7 +1937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1967,7 +1965,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1981,7 +1979,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -1995,7 +1993,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -2009,7 +2007,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -2023,7 +2021,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2037,7 +2035,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2064,9 +2062,9 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
@@ -2080,7 +2078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2108,7 +2106,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -2122,7 +2120,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -2136,7 +2134,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -2159,13 +2157,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA797B3A-3956-4647-86B6-230125BDEE36}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>94</v>
       </c>
@@ -2182,106 +2180,106 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2">
+        <v>2015</v>
+      </c>
+      <c r="C2" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E2" t="s">
         <v>95</v>
       </c>
-      <c r="B2">
-        <v>2011</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3">
+        <v>2015</v>
+      </c>
+      <c r="C3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B4">
+        <v>2017</v>
+      </c>
+      <c r="C4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4" t="s">
+        <v>364</v>
+      </c>
+      <c r="E4" t="s">
         <v>99</v>
       </c>
-      <c r="B3">
-        <v>2012</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B5">
+        <v>2017</v>
+      </c>
+      <c r="C5" t="s">
+        <v>360</v>
+      </c>
+      <c r="D5" t="s">
+        <v>364</v>
+      </c>
+      <c r="E5" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>363</v>
+      </c>
+      <c r="B6">
+        <v>2022</v>
+      </c>
+      <c r="C6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D6" t="s">
+        <v>364</v>
+      </c>
+      <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B7">
+        <v>2022</v>
+      </c>
+      <c r="C7" t="s">
+        <v>360</v>
+      </c>
+      <c r="D7" t="s">
+        <v>364</v>
+      </c>
+      <c r="E7" t="s">
         <v>101</v>
-      </c>
-      <c r="E3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4">
-        <v>2012</v>
-      </c>
-      <c r="C4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5">
-        <v>2012</v>
-      </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6">
-        <v>2018</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7">
-        <v>2018</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2297,9 +2295,9 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2316,41 +2314,41 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="G2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2365,124 +2363,124 @@
         <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>356</v>
+      </c>
+      <c r="B6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>362</v>
-      </c>
-      <c r="B6" t="s">
-        <v>123</v>
-      </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
         <v>120</v>
-      </c>
-      <c r="G8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" t="s">
-        <v>126</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -2494,107 +2492,107 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -2606,84 +2604,84 @@
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
         <v>146</v>
-      </c>
-      <c r="G15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F16" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>150</v>
-      </c>
-      <c r="B17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" t="s">
-        <v>152</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
@@ -2692,50 +2690,50 @@
         <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F18" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
         <v>155</v>
       </c>
-      <c r="G18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
+      <c r="C20" t="s">
         <v>156</v>
-      </c>
-      <c r="B19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F19" t="s">
-        <v>158</v>
-      </c>
-      <c r="G19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>160</v>
-      </c>
-      <c r="B20" t="s">
-        <v>161</v>
-      </c>
-      <c r="C20" t="s">
-        <v>162</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>75</v>
@@ -2747,76 +2745,76 @@
         <v>75</v>
       </c>
       <c r="G20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F22" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="G22" t="s">
         <v>164</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>165</v>
       </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="B23" t="s">
         <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B22" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F22" t="s">
-        <v>169</v>
-      </c>
-      <c r="G22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>171</v>
-      </c>
-      <c r="B23" t="s">
-        <v>172</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="G23" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2832,11 +2830,11 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -2845,343 +2843,343 @@
         <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C2">
         <v>2021</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C3">
         <v>2021</v>
       </c>
       <c r="D3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C4">
         <v>2020</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C5">
         <v>2020</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C6">
         <v>2019</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>2019</v>
       </c>
       <c r="D7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>207</v>
-      </c>
-      <c r="B8" t="s">
-        <v>208</v>
       </c>
       <c r="C8">
         <v>2018</v>
       </c>
       <c r="D8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C9">
         <v>2018</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C10">
         <v>2018</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B11" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="C11">
         <v>2018</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C12">
         <v>2018</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C13">
         <v>2017</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C14">
         <v>2017</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C15">
         <v>2017</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C16">
         <v>2017</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B17" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C17">
         <v>2017</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C18">
         <v>2016</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C19">
         <v>2016</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B20" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C20">
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C21">
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B22" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C22">
         <v>2015</v>
       </c>
       <c r="D22" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" t="s">
         <v>224</v>
-      </c>
-      <c r="B23" t="s">
-        <v>230</v>
       </c>
       <c r="C23">
         <v>2015</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B24" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C24">
         <v>2014</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B25" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C25">
         <v>2014</v>
       </c>
       <c r="D25" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3197,9 +3195,9 @@
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3216,15 +3214,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -3233,21 +3231,21 @@
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="G2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -3256,21 +3254,21 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="G3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -3285,15 +3283,15 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G4" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -3308,15 +3306,15 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G5" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -3331,15 +3329,15 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -3354,15 +3352,15 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -3377,15 +3375,15 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G8" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -3400,15 +3398,15 @@
         <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -3423,84 +3421,84 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B11" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F11" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B12" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -3509,21 +3507,21 @@
         <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G14" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -3532,21 +3530,21 @@
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -3555,21 +3553,21 @@
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -3578,85 +3576,85 @@
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="F17" t="s">
+        <v>251</v>
+      </c>
+      <c r="G17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>256</v>
+      </c>
+      <c r="B18" t="s">
         <v>257</v>
       </c>
-      <c r="G17" t="s">
+      <c r="C18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F18" t="s">
+        <v>259</v>
+      </c>
+      <c r="G18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>262</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F19" t="s">
         <v>263</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G19" t="s">
         <v>264</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B20" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G20" t="s">
         <v>265</v>
-      </c>
-      <c r="G18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>267</v>
-      </c>
-      <c r="B19" t="s">
-        <v>268</v>
-      </c>
-      <c r="C19" t="s">
-        <v>264</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F19" t="s">
-        <v>269</v>
-      </c>
-      <c r="G19" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>267</v>
-      </c>
-      <c r="B20" t="s">
-        <v>268</v>
-      </c>
-      <c r="C20" t="s">
-        <v>264</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F20" t="s">
-        <v>269</v>
-      </c>
-      <c r="G20" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3672,90 +3670,90 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" t="s">
         <v>280</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D2" t="s">
         <v>281</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>282</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="C3" t="s">
         <v>284</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
         <v>285</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>286</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B4" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
         <v>288</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D4" t="s">
         <v>289</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>290</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
         <v>292</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D5" t="s">
         <v>293</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>294</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="C6" t="s">
         <v>296</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D6" t="s">
         <v>297</v>
-      </c>
-      <c r="C5" t="s">
-        <v>298</v>
-      </c>
-      <c r="D5" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>300</v>
-      </c>
-      <c r="B6" t="s">
-        <v>301</v>
-      </c>
-      <c r="C6" t="s">
-        <v>302</v>
-      </c>
-      <c r="D6" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -3771,9 +3769,9 @@
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3790,15 +3788,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -3816,15 +3814,15 @@
         <v>44531</v>
       </c>
       <c r="G2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B3" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -3836,18 +3834,18 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -3859,18 +3857,18 @@
         <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -3882,18 +3880,18 @@
         <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="G5" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -3905,41 +3903,41 @@
         <v>63</v>
       </c>
       <c r="F6" t="s">
+        <v>302</v>
+      </c>
+      <c r="G6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" t="s">
         <v>308</v>
       </c>
-      <c r="G6" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>304</v>
-      </c>
-      <c r="B7" t="s">
-        <v>314</v>
-      </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="G7" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B8" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -3951,18 +3949,18 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B9" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -3974,18 +3972,18 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -3994,21 +3992,21 @@
         <v>69</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F10" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G10" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B11" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -4017,18 +4015,18 @@
         <v>69</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F11" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="G11" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -4037,21 +4035,21 @@
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F12" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="G12" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -4060,44 +4058,44 @@
         <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="G13" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B14" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F14" s="3">
         <v>43070</v>
       </c>
       <c r="G14" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -4109,18 +4107,18 @@
         <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="F15" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -4132,18 +4130,18 @@
         <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="F16" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G16" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -4152,62 +4150,62 @@
         <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="F17" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="G17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>329</v>
+      </c>
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>335</v>
-      </c>
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>340</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F18" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="G18" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F19" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="G19" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>